<commit_message>
remove student from list
</commit_message>
<xml_diff>
--- a/assets/data/student_list.xlsx
+++ b/assets/data/student_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyouh95/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyouh95/UCLA/heoc20grads/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C9E66D-88B4-7B4A-BFCC-6FFE93D4F9A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811DF222-6E2E-8040-A74C-B0C62FB78ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27320" yWindow="0" windowWidth="27320" windowHeight="15360" activeTab="1" xr2:uid="{68969D2F-EA01-6246-8C59-B39E2D845C2D}"/>
+    <workbookView xWindow="-27320" yWindow="460" windowWidth="27320" windowHeight="14900" activeTab="1" xr2:uid="{68969D2F-EA01-6246-8C59-B39E2D845C2D}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>Connie Chang</t>
-  </si>
-  <si>
-    <t>Jenny Lee</t>
   </si>
   <si>
     <t>Kari George</t>
@@ -527,10 +524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A62C86-B33E-A649-8BA8-B901C3461785}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,11 +584,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>